<commit_message>
Finished my detailed Alt analsys
</commit_message>
<xml_diff>
--- a/Excel_Challenge_539 - Total Amount Per Item.xlsx
+++ b/Excel_Challenge_539 - Total Amount Per Item.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA0F04D-2E67-44CC-B87B-2FF65B605F22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9B118A5-23EA-4993-B8B3-4F5B54F14A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -656,11 +656,38 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="975" row="8">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{4BE8A820-9B23-4B63-9A09-BA007018D337}">
+  <we:reference id="wa200003696" version="1.3.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
@@ -988,7 +1015,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F10"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1230,8 +1257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5172D25E-7F91-4593-A4D7-C5057E20B1D6}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1543,45 +1570,120 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I15" cm="1">
+        <f t="array" ref="I15:I23">_xlfn.XLOOKUP(H6,{0,6,11,20},C3:F11,,-1)</f>
+        <v>20.3</v>
+      </c>
+    </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" cm="1">
-        <f t="array" ref="B16:B23">_xlfn.MAP(I3:I10,_xlfn.LAMBDA(_xlpm.x,_xlpm.x*AVERAGEIF(A3:A11,_xlfn.SINGLE(+H10:_xlpm.x),_xlfn.XLOOKUP(_xlpm.x,--_xlfn.TEXTBEFORE(C2:F2,{"-";"+"}),C3:F11,,-1))))</f>
+        <f t="array" ref="B16:B23">_xlfn.MAP(
+    I3:I10,
+    _xlfn.LAMBDA(_xlpm.x,
+        _xlpm.x *
+            AVERAGEIF(
+                A3:A11,
+                _xlfn.SINGLE(+H10:_xlpm.x),
+                _xlfn.XLOOKUP(_xlpm.x, --_xlfn.TEXTBEFORE(C2:F2, {"-";"+"}), C3:F11, , -1)
+            )
+    )
+)</f>
         <v>163.33333333333331</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="E16" cm="1">
+        <f t="array" ref="E16:E23">_xlfn.MAP(
+    I3:I10,
+    _xlfn.LAMBDA(_xlpm.x,
+        1 *
+            AVERAGEIF(
+                A3:A11,
+                _xlfn.SINGLE(+H10:_xlpm.x),
+                _xlfn.XLOOKUP(_xlpm.x, --_xlfn.TEXTBEFORE(C2:F2, {"-";"+"}), C3:F11, , -1)
+            )
+    )
+)</f>
+        <v>16.333333333333332</v>
+      </c>
+      <c r="I16">
+        <v>50.7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>712</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="E17">
+        <v>17.8</v>
+      </c>
+      <c r="I17">
+        <v>19.7</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>1513</v>
       </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="E18">
+        <v>17.8</v>
+      </c>
+      <c r="I18">
+        <v>70.5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>1039.5</v>
       </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="E19">
+        <v>69.3</v>
+      </c>
+      <c r="I19">
+        <v>44.2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>3384</v>
       </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="E20">
+        <v>70.5</v>
+      </c>
+      <c r="I20">
+        <v>86.7</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>2740</v>
       </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="E21">
+        <v>45.666666666666664</v>
+      </c>
+      <c r="I21">
+        <v>13.4</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>263.70000000000005</v>
       </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="E22">
+        <v>87.9</v>
+      </c>
+      <c r="I22">
+        <v>97.6</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>704.40000000000009</v>
+      </c>
+      <c r="E23">
+        <v>88.050000000000011</v>
+      </c>
+      <c r="I23">
+        <v>42.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>